<commit_message>
modified plotting routines to save charts as pdf's
</commit_message>
<xml_diff>
--- a/orepass/initial suite/inputs.xlsx
+++ b/orepass/initial suite/inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\284481c\Documents\R\wasim-2.0\develop\initial suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_studio\wasim-2.0\orepass\initial suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2CA3A3-8958-4E85-B255-AD25C7644E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D26BC8-0816-4A84-A32E-8420F22B9931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -74,12 +74,6 @@
     <t>function() max(1, rnorm(1, 2400, 240))</t>
   </si>
   <si>
-    <t>lhd_travel_empty_delay</t>
-  </si>
-  <si>
-    <t>lhd_get_from_drawpoint_delay</t>
-  </si>
-  <si>
     <t>drawpoint_max_stock</t>
   </si>
   <si>
@@ -116,21 +110,6 @@
     <t>hoist_stock_access_limit</t>
   </si>
   <si>
-    <t>n_lhd</t>
-  </si>
-  <si>
-    <t>lhd_unit_capacity</t>
-  </si>
-  <si>
-    <t>lhd_mttr</t>
-  </si>
-  <si>
-    <t>lhd_mtbf</t>
-  </si>
-  <si>
-    <t>lhd_travel_loaded_delay</t>
-  </si>
-  <si>
     <t>n_conveyor</t>
   </si>
   <si>
@@ -173,13 +152,34 @@
     <t>truck_travel_loaded_delay</t>
   </si>
   <si>
-    <t>lhd_put_to_orepass_feed_hopper_delay</t>
-  </si>
-  <si>
     <t>conveyor_get_from_orepass_feed_hopper_delay</t>
   </si>
   <si>
     <t>conveyor_put_to_orepass_stocks_delay</t>
+  </si>
+  <si>
+    <t>n_bogger</t>
+  </si>
+  <si>
+    <t>bogger_unit_capacity</t>
+  </si>
+  <si>
+    <t>bogger_mttr</t>
+  </si>
+  <si>
+    <t>bogger_mtbf</t>
+  </si>
+  <si>
+    <t>bogger_travel_empty_delay</t>
+  </si>
+  <si>
+    <t>bogger_get_from_drawpoint_delay</t>
+  </si>
+  <si>
+    <t>bogger_travel_loaded_delay</t>
+  </si>
+  <si>
+    <t>bogger_put_to_orepass_feed_hopper_delay</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5:AM7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,112 +1087,112 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Z1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AA1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AB1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AC1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AK1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
         <v>34</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>